<commit_message>
feat: listados updated (not really, just opened ;) )
</commit_message>
<xml_diff>
--- a/data/listados/Beneficiarios/L_B_Puerto Saija.xlsx
+++ b/data/listados/Beneficiarios/L_B_Puerto Saija.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2ef5c481a427bbc/Trabajo/Value Creation Analytics SAS/Clientes/ICESI/Producto 3. TrabajoCampoyAnalisis/3. Listados/Beneficiarios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5420f79c2d515b70/All/PacificoTaskForce/ptfr/data/listados/Beneficiarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="8_{2602C46D-70C0-4041-A90A-4509E702D356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE6D65F6-464D-4462-8C41-80E83F084933}"/>
+  <xr:revisionPtr revIDLastSave="265" documentId="8_{2602C46D-70C0-4041-A90A-4509E702D356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EB680FD-ABB6-4CFF-AD79-96F5DAE3C64F}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja 1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="76">
   <si>
     <t>BENEFICIARIOS</t>
   </si>
@@ -249,13 +250,28 @@
   </si>
   <si>
     <t>Allison Yasmith Quiro Chiripua</t>
+  </si>
+  <si>
+    <t>6-</t>
+  </si>
+  <si>
+    <t>7-</t>
+  </si>
+  <si>
+    <t>9-</t>
+  </si>
+  <si>
+    <t>Muestra Beneficiarios</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -356,15 +372,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -372,6 +379,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -389,6 +399,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6AC6C8E-1727-410D-A159-2A57C1C28D7B}" name="Table2" displayName="Table2" ref="B3:H43" totalsRowShown="0">
+  <autoFilter ref="B3:H43" xr:uid="{A6AC6C8E-1727-410D-A159-2A57C1C28D7B}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E30AE7C1-5AC8-4595-A988-A2755D25B339}" name="#"/>
+    <tableColumn id="2" xr3:uid="{7D998669-6EA5-4944-BDF7-65EA7D542B61}" name="Nombre Completo"/>
+    <tableColumn id="3" xr3:uid="{94F91DC7-188F-42BC-AC53-2628ADB129DC}" name="Documento"/>
+    <tableColumn id="4" xr3:uid="{82465B67-CD5B-4109-91DB-C8BA3635C97A}" name="Edad"/>
+    <tableColumn id="5" xr3:uid="{1C4FE621-FDEB-40C3-9ADD-CD90A14600A0}" name="Grado"/>
+    <tableColumn id="6" xr3:uid="{9B7FD0BD-1745-45C7-BDA0-53065C60E1A0}" name="Etnia"/>
+    <tableColumn id="7" xr3:uid="{F3B455C8-46D5-43A0-821F-124BF4F41F71}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,31 +704,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="2:8">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -722,7 +748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -745,7 +771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -765,7 +791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -788,7 +814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -811,7 +837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -831,7 +857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -854,7 +880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>7</v>
       </c>
@@ -877,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -897,7 +923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>9</v>
       </c>
@@ -917,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -937,7 +963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>11</v>
       </c>
@@ -957,7 +983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>12</v>
       </c>
@@ -980,7 +1006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <v>13</v>
       </c>
@@ -1000,7 +1026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>14</v>
       </c>
@@ -1023,7 +1049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <v>15</v>
       </c>
@@ -1043,7 +1069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <v>16</v>
       </c>
@@ -1066,7 +1092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
         <v>17</v>
       </c>
@@ -1086,7 +1112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>18</v>
       </c>
@@ -1106,7 +1132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>19</v>
       </c>
@@ -1126,7 +1152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <v>20</v>
       </c>
@@ -1146,7 +1172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
         <v>21</v>
       </c>
@@ -1166,7 +1192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <v>22</v>
       </c>
@@ -1186,7 +1212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <v>23</v>
       </c>
@@ -1206,7 +1232,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <v>24</v>
       </c>
@@ -1226,7 +1252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>25</v>
       </c>
@@ -1246,7 +1272,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <v>26</v>
       </c>
@@ -1266,7 +1292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
         <v>27</v>
       </c>
@@ -1286,7 +1312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="3">
         <v>28</v>
       </c>
@@ -1306,7 +1332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
         <v>29</v>
       </c>
@@ -1326,7 +1352,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="3">
         <v>30</v>
       </c>
@@ -1346,7 +1372,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>31</v>
       </c>
@@ -1369,7 +1395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="3">
         <v>32</v>
       </c>
@@ -1388,11 +1414,11 @@
       <c r="G35" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H35" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>33</v>
       </c>
@@ -1415,7 +1441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="3">
         <v>34</v>
       </c>
@@ -1438,7 +1464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>35</v>
       </c>
@@ -1458,7 +1484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" s="3">
         <v>36</v>
       </c>
@@ -1478,7 +1504,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>37</v>
       </c>
@@ -1497,11 +1523,11 @@
       <c r="G40" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H40" s="12" t="s">
+      <c r="H40" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" s="3">
         <v>38</v>
       </c>
@@ -1520,31 +1546,31 @@
       <c r="G41" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H41" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="2:8">
-      <c r="B42" s="10">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
         <v>40</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="5">
         <v>1066891090</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E42" s="4">
         <v>16</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8">
+      <c r="G42" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" s="3">
         <v>41</v>
       </c>
@@ -1564,27 +1590,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="2:8">
-      <c r="B44" s="10">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
         <v>42</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="5">
         <v>1666840261</v>
       </c>
-      <c r="E44" s="11">
+      <c r="E44" s="4">
         <v>18</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8">
+      <c r="G44" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="3">
         <v>43</v>
       </c>
@@ -1603,34 +1629,34 @@
       <c r="G45" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="H45" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="2:8">
-      <c r="B46" s="10">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="5">
         <v>1066842726</v>
       </c>
-      <c r="E46" s="11">
+      <c r="E46" s="4">
         <v>14</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G46" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="9" t="s">
+      <c r="G46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" s="3">
         <v>45</v>
       </c>
@@ -1650,27 +1676,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:8">
-      <c r="B48" s="10">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="2">
         <v>46</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="5">
         <v>1066842233</v>
       </c>
-      <c r="E48" s="11">
+      <c r="E48" s="4">
         <v>14</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G48" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7">
+      <c r="G48" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="3">
         <v>47</v>
       </c>
@@ -1690,27 +1716,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="2:7">
-      <c r="B50" s="10">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
         <v>48</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="5">
         <v>1066842572</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E50" s="4">
         <v>14</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="3">
         <v>49</v>
       </c>
@@ -1730,13 +1756,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="2:7">
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1746,4 +1772,894 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBAA44C2-89C5-41FD-88FC-11E2182A5B89}">
+  <dimension ref="B2:H43"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>1030341043</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>1066843990</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>1066842552</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>1809674882</v>
+      </c>
+      <c r="E7">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8">
+        <v>1066779986</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9">
+        <v>1066842572</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10">
+        <v>1066842214</v>
+      </c>
+      <c r="E10">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>1061773330</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>1147954359</v>
+      </c>
+      <c r="E12">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>1066841659</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>1066842091</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>1066843394</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>1066841531</v>
+      </c>
+      <c r="E16">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>1867991321</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18">
+        <v>1066844095</v>
+      </c>
+      <c r="E18">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19">
+        <v>1066843306</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>1066842966</v>
+      </c>
+      <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <v>1066843151</v>
+      </c>
+      <c r="E21">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>2066843459</v>
+      </c>
+      <c r="E22">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>1066842531</v>
+      </c>
+      <c r="E23">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>1147354954</v>
+      </c>
+      <c r="E24">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <v>1112228042</v>
+      </c>
+      <c r="E25">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26">
+        <v>106684308</v>
+      </c>
+      <c r="E26">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27">
+        <v>1066843281</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28">
+        <v>1059986573</v>
+      </c>
+      <c r="E28">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29">
+        <v>1066842310</v>
+      </c>
+      <c r="E29">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30">
+        <v>1066842233</v>
+      </c>
+      <c r="E30">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31">
+        <v>1147954381</v>
+      </c>
+      <c r="E31">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32">
+        <v>106684665</v>
+      </c>
+      <c r="E32">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33">
+        <v>1066891090</v>
+      </c>
+      <c r="E33">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34">
+        <v>1066841826</v>
+      </c>
+      <c r="E34">
+        <v>16</v>
+      </c>
+      <c r="F34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35">
+        <v>1666840261</v>
+      </c>
+      <c r="E35">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36">
+        <v>1066847173</v>
+      </c>
+      <c r="E36">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>73</v>
+      </c>
+      <c r="G36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37">
+        <v>1151440470</v>
+      </c>
+      <c r="E37">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>1058549135</v>
+      </c>
+      <c r="E38">
+        <v>15</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>1066842432</v>
+      </c>
+      <c r="E39">
+        <v>15</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40">
+        <v>1066842209</v>
+      </c>
+      <c r="E40">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>33</v>
+      </c>
+      <c r="C41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41">
+        <v>1066842341</v>
+      </c>
+      <c r="E41">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>1066840176</v>
+      </c>
+      <c r="E42">
+        <v>18</v>
+      </c>
+      <c r="F42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43">
+        <v>1066839933</v>
+      </c>
+      <c r="E43">
+        <v>18</v>
+      </c>
+      <c r="F43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:H43">
+    <sortCondition ref="F4:F43"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>